<commit_message>
Staged all feedback_forms changes (including new templates and refactor prep)
</commit_message>
<xml_diff>
--- a/feedback_forms/current_versions/dairy_digester_operator_feedback_v003.xlsx
+++ b/feedback_forms/current_versions/dairy_digester_operator_feedback_v003.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tony_local\pycharm\feedback_portal\feedback_forms\current_versions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\local\cursor\feedback_portal\feedback_forms\current_versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C49A8B-79F2-4A81-89BC-D71A9F863F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F75442F-C8AD-4236-B4A3-4EA907C873BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30375" yWindow="1590" windowWidth="21600" windowHeight="11100" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
+    <workbookView xWindow="4877" yWindow="1637" windowWidth="16346" windowHeight="13260" tabRatio="705" activeTab="5" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="6" r:id="rId1"/>
@@ -1181,9 +1181,6 @@
     <t>sector</t>
   </si>
   <si>
-    <t>dairy_digester</t>
-  </si>
-  <si>
     <t>Red (alert) color</t>
   </si>
   <si>
@@ -1629,6 +1626,9 @@
   </si>
   <si>
     <t>jinji_transport_recipient</t>
+  </si>
+  <si>
+    <t>Dairy Digester</t>
   </si>
 </sst>
 </file>
@@ -3353,19 +3353,21 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:U108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="65.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="65.7109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="4.15234375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="65.69140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="4.69140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="65.69140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="4.15234375" style="10" customWidth="1"/>
     <col min="6" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -3389,7 +3391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:21" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.4">
       <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
@@ -3398,7 +3400,7 @@
       <c r="E2" s="21"/>
       <c r="F2" s="50"/>
     </row>
-    <row r="3" spans="2:21" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" s="20" customFormat="1" ht="51" x14ac:dyDescent="0.4">
       <c r="B3" s="47" t="s">
         <v>2</v>
       </c>
@@ -3407,13 +3409,13 @@
       <c r="E3" s="21"/>
       <c r="F3" s="51"/>
     </row>
-    <row r="4" spans="2:21" s="20" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" s="20" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
       <c r="E4" s="23"/>
     </row>
-    <row r="5" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -3437,7 +3439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:21" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" s="24" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="52"/>
       <c r="C6" s="52"/>
       <c r="D6" s="52"/>
@@ -3459,12 +3461,12 @@
       <c r="T6" s="53"/>
       <c r="U6" s="53"/>
     </row>
-    <row r="7" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="U7" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B8" s="54" t="s">
         <v>3</v>
       </c>
@@ -3473,7 +3475,7 @@
       <c r="E8" s="25"/>
       <c r="F8" s="50"/>
     </row>
-    <row r="9" spans="2:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B9" s="55" t="s">
         <v>4</v>
       </c>
@@ -3482,7 +3484,7 @@
       <c r="E9" s="25"/>
       <c r="F9" s="50"/>
     </row>
-    <row r="10" spans="2:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B10" s="56" t="s">
         <v>5</v>
       </c>
@@ -3491,7 +3493,7 @@
       <c r="E10" s="25"/>
       <c r="F10" s="50"/>
     </row>
-    <row r="11" spans="2:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B11" s="54" t="s">
         <v>6</v>
       </c>
@@ -3500,7 +3502,7 @@
       <c r="E11" s="25"/>
       <c r="F11" s="50"/>
     </row>
-    <row r="12" spans="2:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B12" s="54" t="s">
         <v>7</v>
       </c>
@@ -3509,7 +3511,7 @@
       <c r="E12" s="25"/>
       <c r="F12" s="50"/>
     </row>
-    <row r="13" spans="2:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B13" s="54" t="s">
         <v>8</v>
       </c>
@@ -3518,7 +3520,7 @@
       <c r="E13" s="25"/>
       <c r="F13" s="50"/>
     </row>
-    <row r="14" spans="2:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B14" s="54" t="s">
         <v>9</v>
       </c>
@@ -3527,7 +3529,7 @@
       <c r="E14" s="25"/>
       <c r="F14" s="50"/>
     </row>
-    <row r="15" spans="2:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B15" s="57" t="s">
         <v>10</v>
       </c>
@@ -3551,7 +3553,7 @@
       <c r="T15" s="45"/>
       <c r="U15" s="45"/>
     </row>
-    <row r="16" spans="2:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B16" s="54" t="s">
         <v>11</v>
       </c>
@@ -3560,7 +3562,7 @@
       <c r="E16" s="25"/>
       <c r="F16" s="50"/>
     </row>
-    <row r="17" spans="2:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B17" s="58" t="s">
         <v>12</v>
       </c>
@@ -3569,12 +3571,12 @@
       <c r="E17" s="25"/>
       <c r="F17" s="50"/>
     </row>
-    <row r="18" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="U18" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:21" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" s="24" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
@@ -3596,12 +3598,12 @@
       <c r="T19" s="53"/>
       <c r="U19" s="53"/>
     </row>
-    <row r="20" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="U20" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B21" s="54" t="s">
         <v>13</v>
       </c>
@@ -3611,7 +3613,7 @@
       </c>
       <c r="E21" s="54"/>
     </row>
-    <row r="22" spans="2:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B22" s="54" t="s">
         <v>14</v>
       </c>
@@ -3621,7 +3623,7 @@
       </c>
       <c r="E22" s="25"/>
     </row>
-    <row r="23" spans="2:21" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B23" s="54" t="s">
         <v>15</v>
       </c>
@@ -3631,7 +3633,7 @@
       </c>
       <c r="E23" s="25"/>
     </row>
-    <row r="24" spans="2:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B24" s="54" t="s">
         <v>16</v>
       </c>
@@ -3641,7 +3643,7 @@
       </c>
       <c r="E24" s="54"/>
     </row>
-    <row r="25" spans="2:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B25" s="54" t="s">
         <v>17</v>
       </c>
@@ -3651,7 +3653,7 @@
       </c>
       <c r="E25" s="54"/>
     </row>
-    <row r="26" spans="2:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B26" s="54" t="s">
         <v>18</v>
       </c>
@@ -3662,12 +3664,12 @@
       <c r="E26" s="54"/>
       <c r="F26" s="50"/>
     </row>
-    <row r="27" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="U27" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:21" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" s="24" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="52"/>
       <c r="C28" s="52"/>
       <c r="D28" s="52"/>
@@ -3689,12 +3691,12 @@
       <c r="T28" s="53"/>
       <c r="U28" s="53"/>
     </row>
-    <row r="29" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="U29" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:21" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B30" s="35" t="s">
         <v>20</v>
       </c>
@@ -3702,7 +3704,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="2:21" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B31" s="35" t="s">
         <v>22</v>
       </c>
@@ -3710,7 +3712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="2:21" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B32" s="35" t="s">
         <v>24</v>
       </c>
@@ -3718,7 +3720,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:21" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:21" s="11" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B33" s="50" t="s">
         <v>26</v>
       </c>
@@ -3728,7 +3730,7 @@
       </c>
       <c r="E33" s="51"/>
     </row>
-    <row r="34" spans="2:21" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:21" s="11" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B34" s="50" t="s">
         <v>28</v>
       </c>
@@ -3738,7 +3740,7 @@
       </c>
       <c r="E34" s="51"/>
     </row>
-    <row r="35" spans="2:21" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:21" s="11" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B35" s="50" t="s">
         <v>30</v>
       </c>
@@ -3748,12 +3750,12 @@
       </c>
       <c r="E35" s="51"/>
     </row>
-    <row r="36" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="U36" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:21" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:21" s="24" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B37" s="52"/>
       <c r="C37" s="52"/>
       <c r="D37" s="52"/>
@@ -3775,12 +3777,12 @@
       <c r="T37" s="53"/>
       <c r="U37" s="53"/>
     </row>
-    <row r="38" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="U38" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:21" s="11" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:21" s="11" customFormat="1" ht="30.45" x14ac:dyDescent="0.4">
       <c r="B39" s="50" t="s">
         <v>32</v>
       </c>
@@ -3790,14 +3792,14 @@
       </c>
       <c r="E39" s="27"/>
     </row>
-    <row r="40" spans="2:21" s="11" customFormat="1" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:21" s="11" customFormat="1" ht="45.45" x14ac:dyDescent="0.4">
       <c r="B40" s="28" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="51"/>
       <c r="D40" s="62"/>
     </row>
-    <row r="41" spans="2:21" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:21" s="20" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B41" s="28" t="s">
         <v>34</v>
       </c>
@@ -3806,14 +3808,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:21" s="11" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:21" s="11" customFormat="1" ht="30.9" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B42" s="28" t="s">
         <v>35</v>
       </c>
       <c r="C42" s="51"/>
       <c r="D42" s="62"/>
     </row>
-    <row r="43" spans="2:21" s="11" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:21" s="11" customFormat="1" ht="50.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B43" s="28" t="s">
         <v>36</v>
       </c>
@@ -3822,7 +3824,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="2:21" s="11" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:21" s="11" customFormat="1" ht="50.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B44" s="28" t="s">
         <v>38</v>
       </c>
@@ -3831,14 +3833,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="2:21" s="11" customFormat="1" ht="32.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:21" s="11" customFormat="1" ht="16.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B45" s="28" t="s">
         <v>39</v>
       </c>
       <c r="C45" s="51"/>
       <c r="D45" s="63"/>
     </row>
-    <row r="46" spans="2:21" s="11" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:21" s="11" customFormat="1" ht="50.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B46" s="50" t="s">
         <v>40</v>
       </c>
@@ -3847,18 +3849,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="2:21" s="11" customFormat="1" ht="46.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:21" s="11" customFormat="1" ht="45.9" thickTop="1" x14ac:dyDescent="0.4">
       <c r="B47" s="46" t="s">
         <v>41</v>
       </c>
       <c r="D47" s="63"/>
     </row>
-    <row r="48" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="U48" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:21" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:21" s="24" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B49" s="52"/>
       <c r="C49" s="52"/>
       <c r="D49" s="52"/>
@@ -3880,13 +3882,13 @@
       <c r="T49" s="53"/>
       <c r="U49" s="53"/>
     </row>
-    <row r="50" spans="2:21" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:21" s="20" customFormat="1" ht="15.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B50" s="50"/>
       <c r="U50" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:21" s="11" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:21" s="11" customFormat="1" ht="50.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B51" s="50" t="s">
         <v>42</v>
       </c>
@@ -3895,7 +3897,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="2:21" s="11" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:21" s="11" customFormat="1" ht="15.9" thickTop="1" x14ac:dyDescent="0.4">
       <c r="B52" s="50" t="s">
         <v>43</v>
       </c>
@@ -3903,18 +3905,18 @@
         <v>45275.53125</v>
       </c>
     </row>
-    <row r="53" spans="2:21" s="11" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:21" s="11" customFormat="1" ht="30.45" x14ac:dyDescent="0.4">
       <c r="B53" s="50" t="s">
         <v>44</v>
       </c>
       <c r="D53" s="62"/>
     </row>
-    <row r="54" spans="2:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B54" s="51"/>
       <c r="C54" s="51"/>
       <c r="D54" s="51"/>
     </row>
-    <row r="55" spans="2:21" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:21" s="24" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B55" s="52"/>
       <c r="C55" s="52"/>
       <c r="D55" s="52"/>
@@ -3936,12 +3938,12 @@
       <c r="T55" s="53"/>
       <c r="U55" s="53"/>
     </row>
-    <row r="56" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:21" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="U56" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:21" s="11" customFormat="1" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:21" s="11" customFormat="1" ht="45.45" x14ac:dyDescent="0.4">
       <c r="B57" s="28" t="s">
         <v>45</v>
       </c>
@@ -3950,7 +3952,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="2:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B58" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B51) &lt;= 60,
@@ -3966,7 +3968,7 @@
       <c r="C58" s="65"/>
       <c r="D58" s="48"/>
     </row>
-    <row r="59" spans="2:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B59" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B52) &lt;= 60,
@@ -3982,7 +3984,7 @@
       <c r="C59" s="65"/>
       <c r="D59" s="48"/>
     </row>
-    <row r="60" spans="2:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B60" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B53) &lt;= 60,
@@ -3998,7 +4000,7 @@
       <c r="C60" s="65"/>
       <c r="D60" s="48"/>
     </row>
-    <row r="61" spans="2:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B61" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B54) &lt;= 60,
@@ -4014,7 +4016,7 @@
       <c r="C61" s="65"/>
       <c r="D61" s="48"/>
     </row>
-    <row r="62" spans="2:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B62" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B55) &lt;= 60,
@@ -4030,7 +4032,7 @@
       <c r="C62" s="65"/>
       <c r="D62" s="48"/>
     </row>
-    <row r="63" spans="2:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B63" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B56) &lt;= 60,
@@ -4046,7 +4048,7 @@
       <c r="C63" s="65"/>
       <c r="D63" s="48"/>
     </row>
-    <row r="64" spans="2:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:21" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B64" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B57) &lt;= 60,
@@ -4062,7 +4064,7 @@
       <c r="C64" s="65"/>
       <c r="D64" s="48"/>
     </row>
-    <row r="65" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B65" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B58) &lt;= 60,
@@ -4078,7 +4080,7 @@
       <c r="C65" s="65"/>
       <c r="D65" s="48"/>
     </row>
-    <row r="66" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B66" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B59) &lt;= 60,
@@ -4094,7 +4096,7 @@
       <c r="C66" s="65"/>
       <c r="D66" s="48"/>
     </row>
-    <row r="67" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B67" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B60) &lt;= 60,
@@ -4110,7 +4112,7 @@
       <c r="C67" s="65"/>
       <c r="D67" s="48"/>
     </row>
-    <row r="68" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B68" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B61) &lt;= 60,
@@ -4126,7 +4128,7 @@
       <c r="C68" s="65"/>
       <c r="D68" s="48"/>
     </row>
-    <row r="69" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B69" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B62) &lt;= 60,
@@ -4142,7 +4144,7 @@
       <c r="C69" s="65"/>
       <c r="D69" s="48"/>
     </row>
-    <row r="70" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B70" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B63) &lt;= 60,
@@ -4158,7 +4160,7 @@
       <c r="C70" s="65"/>
       <c r="D70" s="48"/>
     </row>
-    <row r="71" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B71" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B64) &lt;= 60,
@@ -4174,7 +4176,7 @@
       <c r="C71" s="65"/>
       <c r="D71" s="48"/>
     </row>
-    <row r="72" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B72" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B65) &lt;= 60,
@@ -4190,7 +4192,7 @@
       <c r="C72" s="65"/>
       <c r="D72" s="48"/>
     </row>
-    <row r="73" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B73" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B66) &lt;= 60,
@@ -4206,7 +4208,7 @@
       <c r="C73" s="65"/>
       <c r="D73" s="48"/>
     </row>
-    <row r="74" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B74" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B67) &lt;= 60,
@@ -4222,7 +4224,7 @@
       <c r="C74" s="65"/>
       <c r="D74" s="48"/>
     </row>
-    <row r="75" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B75" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B68) &lt;= 60,
@@ -4238,7 +4240,7 @@
       <c r="C75" s="65"/>
       <c r="D75" s="48"/>
     </row>
-    <row r="76" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B76" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B69) &lt;= 60,
@@ -4254,7 +4256,7 @@
       <c r="C76" s="65"/>
       <c r="D76" s="48"/>
     </row>
-    <row r="77" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B77" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B70) &lt;= 60,
@@ -4270,7 +4272,7 @@
       <c r="C77" s="65"/>
       <c r="D77" s="48"/>
     </row>
-    <row r="78" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B78" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B71) &lt;= 60,
@@ -4286,7 +4288,7 @@
       <c r="C78" s="65"/>
       <c r="D78" s="48"/>
     </row>
-    <row r="79" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B79" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B72) &lt;= 60,
@@ -4302,7 +4304,7 @@
       <c r="C79" s="65"/>
       <c r="D79" s="48"/>
     </row>
-    <row r="80" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B80" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B73) &lt;= 60,
@@ -4318,7 +4320,7 @@
       <c r="C80" s="65"/>
       <c r="D80" s="48"/>
     </row>
-    <row r="81" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B81" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B74) &lt;= 60,
@@ -4334,7 +4336,7 @@
       <c r="C81" s="65"/>
       <c r="D81" s="48"/>
     </row>
-    <row r="82" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B82" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B75) &lt;= 60,
@@ -4350,7 +4352,7 @@
       <c r="C82" s="65"/>
       <c r="D82" s="48"/>
     </row>
-    <row r="83" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B83" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B76) &lt;= 60,
@@ -4366,7 +4368,7 @@
       <c r="C83" s="65"/>
       <c r="D83" s="48"/>
     </row>
-    <row r="84" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B84" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B77) &lt;= 60,
@@ -4382,7 +4384,7 @@
       <c r="C84" s="65"/>
       <c r="D84" s="48"/>
     </row>
-    <row r="85" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B85" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B78) &lt;= 60,
@@ -4398,7 +4400,7 @@
       <c r="C85" s="65"/>
       <c r="D85" s="48"/>
     </row>
-    <row r="86" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B86" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B79) &lt;= 60,
@@ -4414,7 +4416,7 @@
       <c r="C86" s="65"/>
       <c r="D86" s="48"/>
     </row>
-    <row r="87" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B87" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B80) &lt;= 60,
@@ -4430,7 +4432,7 @@
       <c r="C87" s="65"/>
       <c r="D87" s="48"/>
     </row>
-    <row r="88" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B88" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B81) &lt;= 60,
@@ -4446,7 +4448,7 @@
       <c r="C88" s="65"/>
       <c r="D88" s="48"/>
     </row>
-    <row r="89" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B89" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B82) &lt;= 60,
@@ -4462,7 +4464,7 @@
       <c r="C89" s="65"/>
       <c r="D89" s="48"/>
     </row>
-    <row r="90" spans="2:4" s="11" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:4" s="11" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B90" s="28" t="s">
         <v>47</v>
       </c>
@@ -4471,7 +4473,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="91" spans="2:4" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:4" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.4">
       <c r="B91" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B86) &lt;= 60,
@@ -4488,7 +4490,7 @@
       <c r="C91" s="65"/>
       <c r="D91" s="48"/>
     </row>
-    <row r="92" spans="2:4" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:4" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.4">
       <c r="B92" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B87) &lt;= 60,
@@ -4505,7 +4507,7 @@
       <c r="C92" s="65"/>
       <c r="D92" s="48"/>
     </row>
-    <row r="93" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B93" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B88) &lt;= 60,
@@ -4521,7 +4523,7 @@
       <c r="C93" s="65"/>
       <c r="D93" s="48"/>
     </row>
-    <row r="94" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B94" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B89) &lt;= 60,
@@ -4537,7 +4539,7 @@
       <c r="C94" s="65"/>
       <c r="D94" s="48"/>
     </row>
-    <row r="95" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B95" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B90) &lt;= 60,
@@ -4553,7 +4555,7 @@
       <c r="C95" s="65"/>
       <c r="D95" s="48"/>
     </row>
-    <row r="96" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B96" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B91) &lt;= 60,
@@ -4569,7 +4571,7 @@
       <c r="C96" s="65"/>
       <c r="D96" s="48"/>
     </row>
-    <row r="97" spans="2:4" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:4" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.4">
       <c r="B97" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B92) &lt;= 60,
@@ -4586,7 +4588,7 @@
       <c r="C97" s="65"/>
       <c r="D97" s="48"/>
     </row>
-    <row r="98" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B98" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B93) &lt;= 60,
@@ -4602,7 +4604,7 @@
       <c r="C98" s="65"/>
       <c r="D98" s="48"/>
     </row>
-    <row r="99" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B99" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B94) &lt;= 60,
@@ -4618,7 +4620,7 @@
       <c r="C99" s="65"/>
       <c r="D99" s="48"/>
     </row>
-    <row r="100" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B100" s="64" t="str">
         <f>IF(
   LEN(_carb_only!B95) &lt;= 60,
@@ -4634,37 +4636,37 @@
       <c r="C100" s="65"/>
       <c r="D100" s="48"/>
     </row>
-    <row r="101" spans="2:4" s="11" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:4" s="11" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
       <c r="B101" s="28" t="s">
         <v>48</v>
       </c>
       <c r="D101" s="62"/>
     </row>
-    <row r="102" spans="2:4" s="11" customFormat="1" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:4" s="11" customFormat="1" ht="45.45" x14ac:dyDescent="0.4">
       <c r="B102" s="28" t="s">
         <v>49</v>
       </c>
       <c r="D102" s="62"/>
     </row>
-    <row r="103" spans="2:4" s="11" customFormat="1" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:4" s="11" customFormat="1" ht="45.45" x14ac:dyDescent="0.4">
       <c r="B103" s="28" t="s">
         <v>50</v>
       </c>
       <c r="D103" s="62"/>
     </row>
-    <row r="104" spans="2:4" s="11" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:4" s="11" customFormat="1" ht="30.45" x14ac:dyDescent="0.4">
       <c r="B104" s="28" t="s">
         <v>51</v>
       </c>
       <c r="D104" s="62"/>
     </row>
-    <row r="105" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:4" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="B105" s="51"/>
       <c r="D105" s="29"/>
     </row>
-    <row r="106" spans="2:4" s="30" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="2:4" s="11" customFormat="1" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:4" s="30" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="107" spans="2:4" s="30" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="108" spans="2:4" s="11" customFormat="1" ht="30.45" x14ac:dyDescent="0.4">
       <c r="B108" s="28" t="s">
         <v>52</v>
       </c>
@@ -4715,18 +4717,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="45.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.69140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.69140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="45.69140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" s="12" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="12" t="s">
         <v>53</v>
       </c>
@@ -4734,7 +4736,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="G3" s="2"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -4748,7 +4750,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -4756,15 +4758,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B7" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>57</v>
       </c>
@@ -4772,7 +4774,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="11" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B10" s="14" t="s">
         <v>59</v>
       </c>
@@ -4783,7 +4785,7 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:18" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="11" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B11" s="14" t="s">
         <v>61</v>
       </c>
@@ -4794,7 +4796,7 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:18" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="11" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B12" s="14" t="s">
         <v>63</v>
       </c>
@@ -4805,7 +4807,7 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B13" s="14" t="s">
         <v>65</v>
       </c>
@@ -4816,15 +4818,15 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B14" s="11"/>
       <c r="C14" s="14"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B15" s="11"/>
       <c r="C15" s="14"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B16" s="7" t="s">
         <v>67</v>
       </c>
@@ -4841,7 +4843,7 @@
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.4">
       <c r="G17" s="2"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -4855,7 +4857,7 @@
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>68</v>
       </c>
@@ -4886,7 +4888,7 @@
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
     </row>
-    <row r="19" spans="2:18" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" s="11" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="B19" s="11">
         <v>1</v>
       </c>
@@ -4906,7 +4908,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="2:18" s="11" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" s="11" customFormat="1" ht="102" x14ac:dyDescent="0.4">
       <c r="B20" s="11">
         <v>2</v>
       </c>
@@ -4926,7 +4928,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="2:18" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" s="11" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B21" s="11">
         <v>3</v>
       </c>
@@ -4946,7 +4948,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B22" s="11">
         <v>4</v>
       </c>
@@ -4955,7 +4957,7 @@
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B23" s="11">
         <v>5</v>
       </c>
@@ -4964,7 +4966,7 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B24" s="11">
         <v>6</v>
       </c>
@@ -4973,7 +4975,7 @@
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B25" s="11">
         <v>7</v>
       </c>
@@ -4982,7 +4984,7 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B26" s="11">
         <v>8</v>
       </c>
@@ -4991,7 +4993,7 @@
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B27" s="11">
         <v>9</v>
       </c>
@@ -5000,7 +5002,7 @@
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B28" s="11">
         <v>10</v>
       </c>
@@ -5009,7 +5011,7 @@
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B29" s="11">
         <v>11</v>
       </c>
@@ -5018,7 +5020,7 @@
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B30" s="11">
         <v>12</v>
       </c>
@@ -5027,7 +5029,7 @@
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B31" s="11">
         <v>13</v>
       </c>
@@ -5036,7 +5038,7 @@
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B32" s="11">
         <v>14</v>
       </c>
@@ -5045,7 +5047,7 @@
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B33" s="11">
         <v>15</v>
       </c>
@@ -5054,7 +5056,7 @@
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B34" s="11">
         <v>16</v>
       </c>
@@ -5063,7 +5065,7 @@
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
     </row>
-    <row r="35" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B35" s="11">
         <v>17</v>
       </c>
@@ -5072,7 +5074,7 @@
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
     </row>
-    <row r="36" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B36" s="11">
         <v>18</v>
       </c>
@@ -5081,7 +5083,7 @@
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B37" s="11">
         <v>19</v>
       </c>
@@ -5090,7 +5092,7 @@
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
     </row>
-    <row r="38" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B38" s="11">
         <v>20</v>
       </c>
@@ -5099,7 +5101,7 @@
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B39" s="11">
         <v>21</v>
       </c>
@@ -5108,7 +5110,7 @@
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B40" s="11">
         <v>22</v>
       </c>
@@ -5117,7 +5119,7 @@
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
     </row>
-    <row r="41" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B41" s="11">
         <v>23</v>
       </c>
@@ -5126,7 +5128,7 @@
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
     </row>
-    <row r="42" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B42" s="11">
         <v>24</v>
       </c>
@@ -5135,7 +5137,7 @@
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>
     </row>
-    <row r="43" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B43" s="11">
         <v>25</v>
       </c>
@@ -5144,7 +5146,7 @@
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
     </row>
-    <row r="44" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B44" s="11">
         <v>26</v>
       </c>
@@ -5153,7 +5155,7 @@
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
     </row>
-    <row r="45" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B45" s="11">
         <v>27</v>
       </c>
@@ -5162,7 +5164,7 @@
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
     </row>
-    <row r="46" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B46" s="11">
         <v>28</v>
       </c>
@@ -5171,7 +5173,7 @@
       <c r="F46" s="14"/>
       <c r="G46" s="14"/>
     </row>
-    <row r="47" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B47" s="11">
         <v>29</v>
       </c>
@@ -5180,7 +5182,7 @@
       <c r="F47" s="14"/>
       <c r="G47" s="14"/>
     </row>
-    <row r="48" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B48" s="11">
         <v>30</v>
       </c>
@@ -5189,7 +5191,7 @@
       <c r="F48" s="14"/>
       <c r="G48" s="14"/>
     </row>
-    <row r="49" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B49" s="11">
         <v>31</v>
       </c>
@@ -5198,7 +5200,7 @@
       <c r="F49" s="14"/>
       <c r="G49" s="14"/>
     </row>
-    <row r="50" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B50" s="11">
         <v>32</v>
       </c>
@@ -5207,7 +5209,7 @@
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
     </row>
-    <row r="51" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B51" s="11">
         <v>33</v>
       </c>
@@ -5216,7 +5218,7 @@
       <c r="F51" s="14"/>
       <c r="G51" s="14"/>
     </row>
-    <row r="52" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B52" s="11">
         <v>34</v>
       </c>
@@ -5225,7 +5227,7 @@
       <c r="F52" s="14"/>
       <c r="G52" s="14"/>
     </row>
-    <row r="53" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B53" s="11">
         <v>35</v>
       </c>
@@ -5234,7 +5236,7 @@
       <c r="F53" s="14"/>
       <c r="G53" s="14"/>
     </row>
-    <row r="54" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B54" s="11">
         <v>36</v>
       </c>
@@ -5243,7 +5245,7 @@
       <c r="F54" s="14"/>
       <c r="G54" s="14"/>
     </row>
-    <row r="55" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B55" s="11">
         <v>37</v>
       </c>
@@ -5252,7 +5254,7 @@
       <c r="F55" s="14"/>
       <c r="G55" s="14"/>
     </row>
-    <row r="56" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B56" s="11">
         <v>38</v>
       </c>
@@ -5261,7 +5263,7 @@
       <c r="F56" s="14"/>
       <c r="G56" s="14"/>
     </row>
-    <row r="57" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B57" s="11">
         <v>39</v>
       </c>
@@ -5271,7 +5273,7 @@
       <c r="G57" s="14"/>
       <c r="L57" s="41"/>
     </row>
-    <row r="58" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B58" s="11">
         <v>40</v>
       </c>
@@ -5280,7 +5282,7 @@
       <c r="F58" s="14"/>
       <c r="G58" s="14"/>
     </row>
-    <row r="59" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B59" s="11">
         <v>41</v>
       </c>
@@ -5289,7 +5291,7 @@
       <c r="F59" s="14"/>
       <c r="G59" s="14"/>
     </row>
-    <row r="60" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B60" s="11">
         <v>42</v>
       </c>
@@ -5298,7 +5300,7 @@
       <c r="F60" s="14"/>
       <c r="G60" s="14"/>
     </row>
-    <row r="61" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B61" s="11">
         <v>43</v>
       </c>
@@ -5307,7 +5309,7 @@
       <c r="F61" s="14"/>
       <c r="G61" s="14"/>
     </row>
-    <row r="62" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B62" s="11">
         <v>44</v>
       </c>
@@ -5316,7 +5318,7 @@
       <c r="F62" s="14"/>
       <c r="G62" s="14"/>
     </row>
-    <row r="63" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B63" s="11">
         <v>45</v>
       </c>
@@ -5325,7 +5327,7 @@
       <c r="F63" s="14"/>
       <c r="G63" s="14"/>
     </row>
-    <row r="64" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B64" s="11">
         <v>46</v>
       </c>
@@ -5334,7 +5336,7 @@
       <c r="F64" s="14"/>
       <c r="G64" s="14"/>
     </row>
-    <row r="65" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B65" s="11">
         <v>47</v>
       </c>
@@ -5343,7 +5345,7 @@
       <c r="F65" s="14"/>
       <c r="G65" s="14"/>
     </row>
-    <row r="66" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B66" s="11">
         <v>48</v>
       </c>
@@ -5352,7 +5354,7 @@
       <c r="F66" s="14"/>
       <c r="G66" s="14"/>
     </row>
-    <row r="67" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B67" s="11">
         <v>49</v>
       </c>
@@ -5361,7 +5363,7 @@
       <c r="F67" s="14"/>
       <c r="G67" s="14"/>
     </row>
-    <row r="68" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B68" s="11">
         <v>50</v>
       </c>
@@ -5370,7 +5372,7 @@
       <c r="F68" s="14"/>
       <c r="G68" s="14"/>
     </row>
-    <row r="69" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B69" s="11">
         <v>51</v>
       </c>
@@ -5379,7 +5381,7 @@
       <c r="F69" s="14"/>
       <c r="G69" s="14"/>
     </row>
-    <row r="70" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B70" s="11">
         <v>52</v>
       </c>
@@ -5388,7 +5390,7 @@
       <c r="F70" s="14"/>
       <c r="G70" s="14"/>
     </row>
-    <row r="71" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B71" s="11">
         <v>53</v>
       </c>
@@ -5397,7 +5399,7 @@
       <c r="F71" s="14"/>
       <c r="G71" s="14"/>
     </row>
-    <row r="72" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B72" s="11">
         <v>54</v>
       </c>
@@ -5406,7 +5408,7 @@
       <c r="F72" s="14"/>
       <c r="G72" s="14"/>
     </row>
-    <row r="73" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B73" s="11">
         <v>55</v>
       </c>
@@ -5415,7 +5417,7 @@
       <c r="F73" s="14"/>
       <c r="G73" s="14"/>
     </row>
-    <row r="74" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B74" s="11">
         <v>56</v>
       </c>
@@ -5424,7 +5426,7 @@
       <c r="F74" s="14"/>
       <c r="G74" s="14"/>
     </row>
-    <row r="75" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B75" s="11">
         <v>57</v>
       </c>
@@ -5433,7 +5435,7 @@
       <c r="F75" s="14"/>
       <c r="G75" s="14"/>
     </row>
-    <row r="76" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B76" s="11">
         <v>58</v>
       </c>
@@ -5442,7 +5444,7 @@
       <c r="F76" s="14"/>
       <c r="G76" s="14"/>
     </row>
-    <row r="77" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B77" s="11">
         <v>59</v>
       </c>
@@ -5451,7 +5453,7 @@
       <c r="F77" s="14"/>
       <c r="G77" s="14"/>
     </row>
-    <row r="78" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B78" s="11">
         <v>60</v>
       </c>
@@ -5460,7 +5462,7 @@
       <c r="F78" s="14"/>
       <c r="G78" s="14"/>
     </row>
-    <row r="79" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B79" s="11">
         <v>61</v>
       </c>
@@ -5469,7 +5471,7 @@
       <c r="F79" s="14"/>
       <c r="G79" s="14"/>
     </row>
-    <row r="80" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B80" s="11">
         <v>62</v>
       </c>
@@ -5478,7 +5480,7 @@
       <c r="F80" s="14"/>
       <c r="G80" s="14"/>
     </row>
-    <row r="81" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B81" s="11">
         <v>63</v>
       </c>
@@ -5487,7 +5489,7 @@
       <c r="F81" s="14"/>
       <c r="G81" s="14"/>
     </row>
-    <row r="82" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B82" s="11">
         <v>64</v>
       </c>
@@ -5496,7 +5498,7 @@
       <c r="F82" s="14"/>
       <c r="G82" s="14"/>
     </row>
-    <row r="83" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B83" s="11">
         <v>65</v>
       </c>
@@ -5505,7 +5507,7 @@
       <c r="F83" s="14"/>
       <c r="G83" s="14"/>
     </row>
-    <row r="84" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B84" s="11">
         <v>66</v>
       </c>
@@ -5515,7 +5517,7 @@
       <c r="F84" s="14"/>
       <c r="G84" s="42"/>
     </row>
-    <row r="85" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B85" s="11">
         <v>67</v>
       </c>
@@ -5524,7 +5526,7 @@
       <c r="F85" s="14"/>
       <c r="G85" s="14"/>
     </row>
-    <row r="86" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B86" s="11">
         <v>68</v>
       </c>
@@ -5533,7 +5535,7 @@
       <c r="F86" s="14"/>
       <c r="G86" s="14"/>
     </row>
-    <row r="87" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B87" s="11">
         <v>69</v>
       </c>
@@ -5542,7 +5544,7 @@
       <c r="F87" s="14"/>
       <c r="G87" s="14"/>
     </row>
-    <row r="88" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B88" s="11">
         <v>70</v>
       </c>
@@ -5551,7 +5553,7 @@
       <c r="F88" s="14"/>
       <c r="G88" s="36"/>
     </row>
-    <row r="89" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B89" s="11">
         <v>71</v>
       </c>
@@ -5560,7 +5562,7 @@
       <c r="F89" s="14"/>
       <c r="G89" s="36"/>
     </row>
-    <row r="90" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B90" s="11">
         <v>72</v>
       </c>
@@ -5569,7 +5571,7 @@
       <c r="F90" s="14"/>
       <c r="G90" s="14"/>
     </row>
-    <row r="91" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B91" s="11">
         <v>73</v>
       </c>
@@ -5578,7 +5580,7 @@
       <c r="F91" s="14"/>
       <c r="G91" s="36"/>
     </row>
-    <row r="92" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B92" s="11">
         <v>74</v>
       </c>
@@ -5587,7 +5589,7 @@
       <c r="F92" s="14"/>
       <c r="G92" s="14"/>
     </row>
-    <row r="93" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B93" s="11">
         <v>75</v>
       </c>
@@ -5596,7 +5598,7 @@
       <c r="F93" s="14"/>
       <c r="G93" s="14"/>
     </row>
-    <row r="94" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B94" s="11">
         <v>76</v>
       </c>
@@ -5605,7 +5607,7 @@
       <c r="F94" s="14"/>
       <c r="G94" s="14"/>
     </row>
-    <row r="95" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B95" s="11">
         <v>77</v>
       </c>
@@ -5614,7 +5616,7 @@
       <c r="F95" s="14"/>
       <c r="G95" s="14"/>
     </row>
-    <row r="96" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B96" s="11">
         <v>78</v>
       </c>
@@ -5623,7 +5625,7 @@
       <c r="F96" s="14"/>
       <c r="G96" s="14"/>
     </row>
-    <row r="97" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B97" s="11">
         <v>79</v>
       </c>
@@ -5632,7 +5634,7 @@
       <c r="F97" s="14"/>
       <c r="G97" s="14"/>
     </row>
-    <row r="98" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B98" s="11">
         <v>80</v>
       </c>
@@ -5641,7 +5643,7 @@
       <c r="F98" s="14"/>
       <c r="G98" s="14"/>
     </row>
-    <row r="99" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B99" s="11">
         <v>81</v>
       </c>
@@ -5650,7 +5652,7 @@
       <c r="F99" s="14"/>
       <c r="G99" s="14"/>
     </row>
-    <row r="100" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B100" s="11">
         <v>82</v>
       </c>
@@ -5659,7 +5661,7 @@
       <c r="F100" s="14"/>
       <c r="G100" s="14"/>
     </row>
-    <row r="101" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B101" s="11">
         <v>83</v>
       </c>
@@ -5668,7 +5670,7 @@
       <c r="F101" s="14"/>
       <c r="G101" s="14"/>
     </row>
-    <row r="102" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B102" s="11">
         <v>84</v>
       </c>
@@ -5677,7 +5679,7 @@
       <c r="F102" s="14"/>
       <c r="G102" s="14"/>
     </row>
-    <row r="103" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B103" s="11">
         <v>85</v>
       </c>
@@ -5686,7 +5688,7 @@
       <c r="F103" s="14"/>
       <c r="G103" s="14"/>
     </row>
-    <row r="104" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B104" s="11">
         <v>86</v>
       </c>
@@ -5695,7 +5697,7 @@
       <c r="F104" s="14"/>
       <c r="G104" s="14"/>
     </row>
-    <row r="105" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B105" s="11">
         <v>87</v>
       </c>
@@ -5705,7 +5707,7 @@
       <c r="F105" s="14"/>
       <c r="G105" s="14"/>
     </row>
-    <row r="106" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B106" s="11">
         <v>88</v>
       </c>
@@ -5715,7 +5717,7 @@
       <c r="F106" s="14"/>
       <c r="G106" s="14"/>
     </row>
-    <row r="107" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B107" s="11">
         <v>89</v>
       </c>
@@ -5725,7 +5727,7 @@
       <c r="F107" s="14"/>
       <c r="G107" s="14"/>
     </row>
-    <row r="108" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B108" s="11">
         <v>90</v>
       </c>
@@ -5735,7 +5737,7 @@
       <c r="F108" s="14"/>
       <c r="G108" s="14"/>
     </row>
-    <row r="109" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B109" s="11">
         <v>91</v>
       </c>
@@ -5745,7 +5747,7 @@
       <c r="F109" s="14"/>
       <c r="G109" s="14"/>
     </row>
-    <row r="110" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B110" s="11">
         <v>92</v>
       </c>
@@ -5755,7 +5757,7 @@
       <c r="F110" s="14"/>
       <c r="G110" s="14"/>
     </row>
-    <row r="111" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B111" s="11">
         <v>93</v>
       </c>
@@ -5764,7 +5766,7 @@
       <c r="F111" s="14"/>
       <c r="G111" s="14"/>
     </row>
-    <row r="112" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B112" s="11">
         <v>94</v>
       </c>
@@ -5774,7 +5776,7 @@
       <c r="F112" s="14"/>
       <c r="G112" s="14"/>
     </row>
-    <row r="113" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B113" s="11">
         <v>95</v>
       </c>
@@ -5784,7 +5786,7 @@
       <c r="F113" s="14"/>
       <c r="G113" s="14"/>
     </row>
-    <row r="114" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B114" s="11">
         <v>96</v>
       </c>
@@ -5794,7 +5796,7 @@
       <c r="F114" s="14"/>
       <c r="G114" s="14"/>
     </row>
-    <row r="115" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B115" s="11">
         <v>97</v>
       </c>
@@ -5804,7 +5806,7 @@
       <c r="F115" s="14"/>
       <c r="G115" s="14"/>
     </row>
-    <row r="116" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B116" s="11">
         <v>98</v>
       </c>
@@ -5814,7 +5816,7 @@
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
     </row>
-    <row r="117" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B117" s="11">
         <v>99</v>
       </c>
@@ -5824,7 +5826,7 @@
       <c r="F117" s="14"/>
       <c r="G117" s="14"/>
     </row>
-    <row r="118" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:7" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B118" s="11">
         <v>100</v>
       </c>
@@ -5859,21 +5861,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="92.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" customWidth="1"/>
-    <col min="4" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="17" width="16.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" customWidth="1"/>
+    <col min="2" max="2" width="92.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.15234375" customWidth="1"/>
+    <col min="4" max="5" width="16.69140625" customWidth="1"/>
+    <col min="6" max="17" width="16.69140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" s="38" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" s="38" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="38" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -5893,7 +5895,7 @@
       <c r="P4"/>
       <c r="Q4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -5912,7 +5914,7 @@
       <c r="P5"/>
       <c r="Q5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -5931,7 +5933,7 @@
       <c r="P6"/>
       <c r="Q6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -5944,150 +5946,150 @@
       <c r="P7"/>
       <c r="Q7"/>
     </row>
-    <row r="10" spans="1:17" s="39" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" s="39" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="39" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B19" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B20" s="7"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B34" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B44" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
         <v>113</v>
       </c>
@@ -6103,7 +6105,7 @@
       <c r="P46"/>
       <c r="Q46"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
         <v>114</v>
       </c>
@@ -6118,253 +6120,253 @@
       <c r="P47"/>
       <c r="Q47"/>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.4">
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B49" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B50" s="7"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B55" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B72" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B73" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B82" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B83" s="7"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B84" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B85" s="7"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B86" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B87" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B88" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B89" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B90" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B91" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B92" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B93" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B94" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B95" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B96" s="7"/>
     </row>
-    <row r="97" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:17" x14ac:dyDescent="0.4">
       <c r="G97"/>
     </row>
-    <row r="98" spans="2:17" s="39" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:17" s="39" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B98" s="39" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="99" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:17" x14ac:dyDescent="0.4">
       <c r="G99"/>
     </row>
-    <row r="100" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B100" s="8" t="s">
         <v>160</v>
       </c>
@@ -6372,13 +6374,13 @@
       <c r="F100"/>
       <c r="Q100"/>
     </row>
-    <row r="101" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B101" s="7"/>
       <c r="E101" s="3"/>
       <c r="F101"/>
       <c r="Q101"/>
     </row>
-    <row r="102" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B102" t="s">
         <v>37</v>
       </c>
@@ -6386,7 +6388,7 @@
       <c r="F102"/>
       <c r="Q102"/>
     </row>
-    <row r="103" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B103" t="str" cm="1">
         <f t="array" ref="B103:B106">_carb_only_table_01[]</f>
         <v>An intentional or allowable vent (i.e. the operator was aware of, and/or would not repair)</v>
@@ -6395,7 +6397,7 @@
       <c r="F103"/>
       <c r="Q103"/>
     </row>
-    <row r="104" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B104" t="str">
         <v>An unintentional leak (i.e. the operator was not aware of, and could be repaired if discovered)</v>
       </c>
@@ -6403,7 +6405,7 @@
       <c r="F104"/>
       <c r="Q104"/>
     </row>
-    <row r="105" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B105" t="str">
         <v>Due to a temporary activity (i.e. would be resolved without corrective action when the activity is completed)</v>
       </c>
@@ -6411,7 +6413,7 @@
       <c r="F105"/>
       <c r="Q105"/>
     </row>
-    <row r="106" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B106" t="str">
         <v>Operator was aware of the leak prior to receiving the CARB plume notification and/or repairs were in progress</v>
       </c>
@@ -6419,27 +6421,27 @@
       <c r="F106"/>
       <c r="Q106"/>
     </row>
-    <row r="107" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:17" x14ac:dyDescent="0.4">
       <c r="E107" s="3"/>
       <c r="F107"/>
       <c r="Q107"/>
     </row>
-    <row r="108" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:17" x14ac:dyDescent="0.4">
       <c r="E108" s="3"/>
       <c r="F108"/>
       <c r="Q108"/>
     </row>
-    <row r="109" spans="2:17" s="39" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:17" s="39" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B109" s="39" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="110" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:17" x14ac:dyDescent="0.4">
       <c r="E110" s="3"/>
       <c r="F110"/>
       <c r="Q110"/>
     </row>
-    <row r="111" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B111" s="8" t="s">
         <v>160</v>
       </c>
@@ -6447,89 +6449,89 @@
       <c r="F111"/>
       <c r="Q111"/>
     </row>
-    <row r="112" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B112" s="7"/>
       <c r="E112" s="3"/>
       <c r="F112"/>
       <c r="Q112"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B113" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B114" t="str" cm="1">
         <f t="array" ref="B114:B125">_carb_only_table_02[]</f>
         <v>Animal housing/barn/corral/lot</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B115" t="str">
         <v>Biogas conditioning/upgrading equipment</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B116" t="str">
         <v>Biogas moving/handling equipment</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B117" t="str">
         <v>Digester cover</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B118" t="str">
         <v>Effluent pond</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B119" t="str">
         <v>Interconnection/pipeline</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B120" t="str">
         <v>Manure collection pit</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B121" t="str">
         <v>Manure separator</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B122" t="str">
         <v>Open lagoon</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B123" t="str">
         <v xml:space="preserve">Other </v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B124" t="str">
         <v>Other digester component</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B125" t="str">
         <v>Stacking slab/stockpile/other manure storage</v>
       </c>
     </row>
-    <row r="128" spans="2:2" s="39" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:2" s="39" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B128" s="39" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="129" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:17" x14ac:dyDescent="0.4">
       <c r="E129" s="3"/>
       <c r="F129"/>
       <c r="Q129"/>
     </row>
-    <row r="130" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B130" s="8" t="s">
         <v>160</v>
       </c>
@@ -6537,64 +6539,64 @@
       <c r="F130"/>
       <c r="Q130"/>
     </row>
-    <row r="131" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B131" s="7"/>
       <c r="E131" s="3"/>
       <c r="F131"/>
       <c r="Q131"/>
     </row>
-    <row r="132" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B132" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="133" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B133" t="str" cm="1">
         <f t="array" ref="B133:B139">_carb_only_table_03[]</f>
         <v>Construction activity</v>
       </c>
     </row>
-    <row r="134" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B134" t="str">
         <v>Damaged/broken component (e.g. tear in digester cover, loose flange/port/seal)</v>
       </c>
     </row>
-    <row r="135" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B135" t="str">
         <v>Maintenance/repair/testing activity</v>
       </c>
     </row>
-    <row r="136" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B136" t="str">
         <v>Manure management activity</v>
       </c>
     </row>
-    <row r="137" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B137" t="str">
         <v>Other</v>
       </c>
     </row>
-    <row r="138" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B138" t="str">
         <v>Venting-emergency/temporary</v>
       </c>
     </row>
-    <row r="139" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B139" t="str">
         <v>Venting-intentional/routine</v>
       </c>
     </row>
-    <row r="142" spans="2:17" s="39" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:17" s="39" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B142" s="39" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="143" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:17" x14ac:dyDescent="0.4">
       <c r="E143" s="3"/>
       <c r="F143"/>
       <c r="Q143"/>
     </row>
-    <row r="144" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B144" s="8" t="s">
         <v>160</v>
       </c>
@@ -6602,39 +6604,39 @@
       <c r="F144"/>
       <c r="Q144"/>
     </row>
-    <row r="145" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B145" s="7"/>
       <c r="E145" s="3"/>
       <c r="F145"/>
       <c r="Q145"/>
     </row>
-    <row r="146" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B146" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="147" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B147" t="str" cm="1">
         <f t="array" ref="B147:B148">_carb_only_table_04[]</f>
         <v>Yes</v>
       </c>
     </row>
-    <row r="148" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B148" t="str">
         <v>No</v>
       </c>
     </row>
-    <row r="151" spans="2:17" s="39" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:17" s="39" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B151" s="39" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="152" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:17" x14ac:dyDescent="0.4">
       <c r="E152" s="3"/>
       <c r="F152"/>
       <c r="Q152"/>
     </row>
-    <row r="153" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B153" s="8" t="s">
         <v>160</v>
       </c>
@@ -6642,189 +6644,189 @@
       <c r="F153"/>
       <c r="Q153"/>
     </row>
-    <row r="154" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B154" s="7"/>
       <c r="E154" s="3"/>
       <c r="F154"/>
       <c r="Q154"/>
     </row>
-    <row r="155" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B155" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="156" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B156" t="str" cm="1">
         <f t="array" ref="B156:B187">_carb_only_table_05[]</f>
         <v>Advanced solid-liquid separation by flocculation</v>
       </c>
     </row>
-    <row r="157" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B157" t="str">
         <v>Anaerobic digester</v>
       </c>
     </row>
-    <row r="158" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B158" t="str">
         <v>Anaerobic Lagoon</v>
       </c>
     </row>
-    <row r="159" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B159" t="str">
         <v>Centrifuge/decanter</v>
       </c>
     </row>
-    <row r="160" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B160" t="str">
         <v>Compost bedded pack barn</v>
       </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B161" t="str">
         <v>Composting aerated</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B162" t="str">
         <v>Composting in vessel</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B163" t="str">
         <v>Composting windrows</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B164" t="str">
         <v>Daily spread</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B165" t="str">
         <v>Dry lot/corral</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B166" t="str">
         <v>Fertigation</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B167" t="str">
         <v>Land application (flood)</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B168" t="str">
         <v>Land application (subsurface drip)</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B169" t="str">
         <v>Liquid/flush manure collection</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B170" t="str">
         <v>Liquid/slurry</v>
       </c>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B171" t="str">
         <v>Other mechanical solid-liquid separator</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B172" t="str">
         <v>Pasture</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B173" t="str">
         <v>Processing pit</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B174" t="str">
         <v>Roller drum separator</v>
       </c>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B175" t="str">
         <v>Sand lane</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B176" t="str">
         <v>Screw press separator</v>
       </c>
     </row>
-    <row r="177" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B177" t="str">
         <v>Settling basin</v>
       </c>
     </row>
-    <row r="178" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B178" t="str">
         <v>Slatted floor pit storage</v>
       </c>
     </row>
-    <row r="179" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B179" t="str">
         <v>Sloped screen separator</v>
       </c>
     </row>
-    <row r="180" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B180" t="str">
         <v>Solar drying</v>
       </c>
     </row>
-    <row r="181" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B181" t="str">
         <v>Solid storage</v>
       </c>
     </row>
-    <row r="182" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B182" t="str">
         <v>Solid/dry scrape manure collection</v>
       </c>
     </row>
-    <row r="183" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B183" t="str">
         <v>Stationary screen separator</v>
       </c>
     </row>
-    <row r="184" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B184" t="str">
         <v>Vacuum manure collection</v>
       </c>
     </row>
-    <row r="185" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B185" t="str">
         <v>Vermifiltration</v>
       </c>
     </row>
-    <row r="186" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B186" t="str">
         <v>Vibrating screen separator</v>
       </c>
     </row>
-    <row r="187" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B187" t="str">
         <v>Weeping wall</v>
       </c>
     </row>
-    <row r="190" spans="2:17" s="39" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:17" s="39" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B190" s="39" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="191" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:17" x14ac:dyDescent="0.4">
       <c r="E191" s="3"/>
       <c r="F191"/>
       <c r="Q191"/>
     </row>
-    <row r="192" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B192" s="8" t="s">
         <v>160</v>
       </c>
@@ -6832,64 +6834,64 @@
       <c r="F192"/>
       <c r="Q192"/>
     </row>
-    <row r="193" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B193" s="7"/>
       <c r="E193" s="3"/>
       <c r="F193"/>
       <c r="Q193"/>
     </row>
-    <row r="194" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B194" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="195" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B195" t="str" cm="1">
         <f t="array" ref="B195:B204">_carb_only_table_06[]</f>
         <v>Biogas conditioning (e.g. hydrogen sulfide moisture particulate removal)</v>
       </c>
     </row>
-    <row r="196" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B196" t="str">
         <v>Biogas moving and handling equipement (e.g. blower collection box pre-conditioning gas pipelines)</v>
       </c>
     </row>
-    <row r="197" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B197" t="str">
         <v>Biomethane upgrading</v>
       </c>
     </row>
-    <row r="198" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B198" t="str">
         <v>Covered lagoon anaerobic digester</v>
       </c>
     </row>
-    <row r="199" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B199" t="str">
         <v>Electricity generation</v>
       </c>
     </row>
-    <row r="200" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B200" t="str">
         <v>Heating/process fuel equipment</v>
       </c>
     </row>
-    <row r="201" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B201" t="str">
         <v>Interconnection point of receipt (including biomethane quality testing)</v>
       </c>
     </row>
-    <row r="202" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B202" t="str">
         <v>In-vessel anaerobic digester</v>
       </c>
     </row>
-    <row r="203" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B203" t="str">
         <v>Onsite fuel use or dispensing</v>
       </c>
     </row>
-    <row r="204" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B204" t="str">
         <v>Pipeline lateral</v>
       </c>
@@ -6915,19 +6917,19 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="9" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" customWidth="1"/>
+    <col min="2" max="3" width="30.69140625" customWidth="1"/>
+    <col min="4" max="9" width="8.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" s="5" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -6935,7 +6937,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -6943,7 +6945,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -6951,7 +6953,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -6959,7 +6961,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="6" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="6" t="s">
         <v>171</v>
       </c>
@@ -6967,7 +6969,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>173</v>
       </c>
@@ -6985,20 +6987,22 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:C16"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="3" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" customWidth="1"/>
+    <col min="2" max="3" width="30.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" s="5" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -7006,7 +7010,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -7014,7 +7018,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -7022,7 +7026,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -7030,12 +7034,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:3" s="6" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="6" t="s">
         <v>178</v>
       </c>
@@ -7043,20 +7047,20 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>180</v>
       </c>
       <c r="C15" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>182</v>
-      </c>
-      <c r="C16" t="s">
-        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -7070,425 +7074,446 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:F81"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:F81"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" customWidth="1"/>
+    <col min="2" max="2" width="25.15234375" customWidth="1"/>
+    <col min="3" max="3" width="16.3828125" customWidth="1"/>
+    <col min="4" max="4" width="51.84375" customWidth="1"/>
+    <col min="5" max="5" width="16.3828125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="99" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="12" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2" s="13"/>
       <c r="F2" s="16"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C4" s="1"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C5" s="1"/>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C6" s="1"/>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C7" s="1"/>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C8" s="1"/>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" s="6" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="6" t="s">
         <v>171</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>173</v>
       </c>
       <c r="C11" t="s">
-        <v>202</v>
-      </c>
-      <c r="D11" t="s">
-        <v>237</v>
+        <v>260</v>
+      </c>
+      <c r="D11" s="66" t="s">
+        <v>261</v>
       </c>
       <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>173</v>
       </c>
       <c r="C12" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="D12" t="s">
-        <v>190</v>
+        <v>241</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>173</v>
       </c>
       <c r="C13" t="s">
-        <v>238</v>
+        <v>326</v>
       </c>
       <c r="D13" t="s">
-        <v>239</v>
+        <v>327</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>173</v>
       </c>
       <c r="C14" t="s">
-        <v>240</v>
+        <v>328</v>
       </c>
       <c r="D14" t="s">
-        <v>192</v>
+        <v>329</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>173</v>
       </c>
       <c r="C15" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D15" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>173</v>
       </c>
       <c r="C16" t="s">
-        <v>243</v>
-      </c>
-      <c r="D16" s="66" t="s">
-        <v>244</v>
+        <v>239</v>
+      </c>
+      <c r="D16" t="s">
+        <v>191</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>173</v>
       </c>
       <c r="C17" t="s">
-        <v>245</v>
-      </c>
-      <c r="D17" s="66" t="s">
-        <v>246</v>
+        <v>268</v>
+      </c>
+      <c r="D17" t="s">
+        <v>209</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>173</v>
       </c>
       <c r="C18" t="s">
-        <v>247</v>
-      </c>
-      <c r="D18" s="66" t="s">
-        <v>248</v>
+        <v>269</v>
+      </c>
+      <c r="D18" t="s">
+        <v>212</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
         <v>173</v>
       </c>
       <c r="C19" t="s">
-        <v>249</v>
-      </c>
-      <c r="D19" s="66" t="s">
-        <v>250</v>
+        <v>208</v>
+      </c>
+      <c r="D19" t="s">
+        <v>231</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="18">
+        <v>45468</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>173</v>
       </c>
       <c r="C20" t="s">
-        <v>251</v>
-      </c>
-      <c r="D20" s="66" t="s">
-        <v>252</v>
+        <v>211</v>
+      </c>
+      <c r="D20" t="s">
+        <v>224</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>35.321100000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>173</v>
       </c>
       <c r="C21" t="s">
-        <v>253</v>
-      </c>
-      <c r="D21" s="66" t="s">
-        <v>254</v>
+        <v>230</v>
+      </c>
+      <c r="D21" t="s">
+        <v>225</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>-119.5808</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
         <v>173</v>
       </c>
       <c r="C22" t="s">
-        <v>255</v>
-      </c>
-      <c r="D22" s="66" t="s">
-        <v>256</v>
+        <v>223</v>
+      </c>
+      <c r="D22" t="s">
+        <v>210</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>173</v>
       </c>
       <c r="C23" t="s">
-        <v>257</v>
-      </c>
-      <c r="D23" s="66" t="s">
-        <v>258</v>
+        <v>262</v>
+      </c>
+      <c r="D23" t="s">
+        <v>263</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>173</v>
       </c>
       <c r="C24" t="s">
-        <v>259</v>
-      </c>
-      <c r="D24" s="66" t="s">
-        <v>260</v>
+        <v>271</v>
+      </c>
+      <c r="D24" t="s">
+        <v>272</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>173</v>
       </c>
       <c r="C25" t="s">
-        <v>261</v>
-      </c>
-      <c r="D25" s="66" t="s">
-        <v>262</v>
+        <v>206</v>
+      </c>
+      <c r="D25" t="s">
+        <v>267</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>173</v>
       </c>
       <c r="C26" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="D26" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>173</v>
       </c>
       <c r="C27" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="D27" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>173</v>
       </c>
       <c r="C28" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D28" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>173</v>
       </c>
       <c r="C29" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="D29" t="s">
-        <v>264</v>
+        <v>218</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
       </c>
-      <c r="F29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="67">
+        <v>45152.53125</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>173</v>
       </c>
       <c r="C30" t="s">
-        <v>265</v>
+        <v>217</v>
       </c>
       <c r="D30" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="E30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>173</v>
       </c>
       <c r="C31" t="s">
+        <v>219</v>
+      </c>
+      <c r="D31" t="s">
         <v>216</v>
-      </c>
-      <c r="D31" t="s">
-        <v>200</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>173</v>
       </c>
       <c r="C32" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="D32" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="E32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>173</v>
       </c>
       <c r="C33" t="s">
-        <v>267</v>
+        <v>188</v>
       </c>
       <c r="D33" t="s">
         <v>205</v>
       </c>
       <c r="E33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
         <v>173</v>
       </c>
       <c r="C34" t="s">
-        <v>189</v>
+        <v>265</v>
       </c>
       <c r="D34" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E34" t="b">
         <v>1</v>
@@ -7497,689 +7522,668 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>173</v>
       </c>
       <c r="C35" t="s">
-        <v>207</v>
+        <v>266</v>
       </c>
       <c r="D35" t="s">
-        <v>268</v>
+        <v>204</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
       </c>
-      <c r="F35" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
         <v>173</v>
       </c>
       <c r="C36" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D36" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E36" t="b">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>173</v>
       </c>
       <c r="C37" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D37" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
       </c>
-      <c r="F37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>173</v>
       </c>
       <c r="C38" t="s">
-        <v>270</v>
+        <v>201</v>
       </c>
       <c r="D38" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="E38" t="b">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>173</v>
       </c>
       <c r="C39" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="D39" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="67">
+        <v>45275.53125</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>173</v>
       </c>
       <c r="C40" t="s">
-        <v>271</v>
+        <v>197</v>
       </c>
       <c r="D40" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
       </c>
-      <c r="F40" s="67">
-        <v>45152.53125</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>173</v>
       </c>
       <c r="C41" t="s">
-        <v>201</v>
+        <v>273</v>
       </c>
       <c r="D41" t="s">
-        <v>221</v>
+        <v>274</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>173</v>
       </c>
       <c r="C42" t="s">
-        <v>212</v>
-      </c>
-      <c r="D42" t="s">
-        <v>225</v>
+        <v>275</v>
+      </c>
+      <c r="D42" s="66" t="s">
+        <v>276</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
       </c>
-      <c r="F42">
-        <v>35.321100000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
         <v>173</v>
       </c>
       <c r="C43" t="s">
-        <v>272</v>
-      </c>
-      <c r="D43" t="s">
-        <v>273</v>
+        <v>226</v>
+      </c>
+      <c r="D43" s="66" t="s">
+        <v>277</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
       </c>
-      <c r="F43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
         <v>173</v>
       </c>
       <c r="C44" t="s">
-        <v>231</v>
-      </c>
-      <c r="D44" t="s">
-        <v>226</v>
+        <v>228</v>
+      </c>
+      <c r="D44" s="66" t="s">
+        <v>278</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
       </c>
-      <c r="F44">
-        <v>-119.5808</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
         <v>173</v>
       </c>
       <c r="C45" t="s">
-        <v>274</v>
-      </c>
-      <c r="D45" t="s">
-        <v>275</v>
+        <v>235</v>
+      </c>
+      <c r="D45" s="66" t="s">
+        <v>279</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
         <v>173</v>
       </c>
       <c r="C46" t="s">
-        <v>276</v>
+        <v>234</v>
       </c>
       <c r="D46" s="66" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
         <v>173</v>
       </c>
       <c r="C47" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="D47" s="66" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B48" t="s">
         <v>173</v>
       </c>
       <c r="C48" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="D48" s="66" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B49" t="s">
         <v>173</v>
       </c>
       <c r="C49" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D49" s="66" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
         <v>173</v>
       </c>
       <c r="C50" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D50" s="66" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
         <v>173</v>
       </c>
       <c r="C51" t="s">
-        <v>214</v>
+        <v>285</v>
       </c>
       <c r="D51" s="66" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
         <v>173</v>
       </c>
       <c r="C52" t="s">
-        <v>215</v>
+        <v>287</v>
       </c>
       <c r="D52" s="66" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
         <v>173</v>
       </c>
       <c r="C53" t="s">
-        <v>233</v>
+        <v>289</v>
       </c>
       <c r="D53" s="66" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
         <v>173</v>
       </c>
       <c r="C54" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="D54" s="66" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B55" t="s">
         <v>173</v>
       </c>
       <c r="C55" t="s">
-        <v>286</v>
+        <v>221</v>
       </c>
       <c r="D55" s="66" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
         <v>173</v>
       </c>
       <c r="C56" t="s">
-        <v>288</v>
+        <v>190</v>
       </c>
       <c r="D56" s="66" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="E56" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
         <v>173</v>
       </c>
       <c r="C57" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D57" s="66" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="E57" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
         <v>173</v>
       </c>
       <c r="C58" t="s">
-        <v>223</v>
+        <v>296</v>
       </c>
       <c r="D58" s="66" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="E58" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
         <v>173</v>
       </c>
       <c r="C59" t="s">
-        <v>222</v>
+        <v>298</v>
       </c>
       <c r="D59" s="66" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
         <v>173</v>
       </c>
       <c r="C60" t="s">
-        <v>191</v>
+        <v>300</v>
       </c>
       <c r="D60" s="66" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="E60" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
         <v>173</v>
       </c>
       <c r="C61" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="D61" s="66" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
         <v>173</v>
       </c>
       <c r="C62" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D62" s="66" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="E62" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
         <v>173</v>
       </c>
       <c r="C63" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="D63" s="66" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="E63" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
         <v>173</v>
       </c>
       <c r="C64" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="D64" s="66" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="E64" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
         <v>173</v>
       </c>
       <c r="C65" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="D65" s="66" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="E65" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
         <v>173</v>
       </c>
       <c r="C66" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="D66" s="66" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="E66" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
         <v>173</v>
       </c>
       <c r="C67" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="D67" s="66" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="E67" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
         <v>173</v>
       </c>
       <c r="C68" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="D68" s="66" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="E68" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
         <v>173</v>
       </c>
       <c r="C69" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="D69" s="66" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
         <v>173</v>
       </c>
       <c r="C70" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="D70" s="66" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="E70" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
         <v>173</v>
       </c>
       <c r="C71" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="D71" s="66" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="E71" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B72" t="s">
         <v>173</v>
       </c>
       <c r="C72" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="D72" s="66" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="E72" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B73" t="s">
         <v>173</v>
       </c>
       <c r="C73" t="s">
-        <v>319</v>
+        <v>242</v>
       </c>
       <c r="D73" s="66" t="s">
-        <v>320</v>
+        <v>243</v>
       </c>
       <c r="E73" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
         <v>173</v>
       </c>
       <c r="C74" t="s">
-        <v>321</v>
+        <v>244</v>
       </c>
       <c r="D74" s="66" t="s">
-        <v>322</v>
+        <v>245</v>
       </c>
       <c r="E74" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
         <v>173</v>
       </c>
       <c r="C75" t="s">
-        <v>323</v>
+        <v>246</v>
       </c>
       <c r="D75" s="66" t="s">
-        <v>324</v>
+        <v>247</v>
       </c>
       <c r="E75" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
         <v>173</v>
       </c>
       <c r="C76" t="s">
-        <v>325</v>
+        <v>248</v>
       </c>
       <c r="D76" s="66" t="s">
-        <v>326</v>
+        <v>249</v>
       </c>
       <c r="E76" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
         <v>173</v>
       </c>
       <c r="C77" t="s">
-        <v>198</v>
-      </c>
-      <c r="D77" t="s">
-        <v>228</v>
+        <v>250</v>
+      </c>
+      <c r="D77" s="66" t="s">
+        <v>251</v>
       </c>
       <c r="E77" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
         <v>173</v>
       </c>
       <c r="C78" t="s">
-        <v>204</v>
-      </c>
-      <c r="D78" t="s">
-        <v>230</v>
+        <v>252</v>
+      </c>
+      <c r="D78" s="66" t="s">
+        <v>253</v>
       </c>
       <c r="E78" t="b">
         <v>0</v>
       </c>
-      <c r="F78" s="67">
-        <v>45275.53125</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
         <v>173</v>
       </c>
       <c r="C79" t="s">
-        <v>209</v>
-      </c>
-      <c r="D79" t="s">
-        <v>232</v>
+        <v>256</v>
+      </c>
+      <c r="D79" s="66" t="s">
+        <v>257</v>
       </c>
       <c r="E79" t="b">
         <v>0</v>
       </c>
-      <c r="F79" s="18">
-        <v>45468</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
         <v>173</v>
       </c>
       <c r="C80" t="s">
-        <v>327</v>
-      </c>
-      <c r="D80" t="s">
-        <v>328</v>
+        <v>254</v>
+      </c>
+      <c r="D80" s="66" t="s">
+        <v>255</v>
       </c>
       <c r="E80" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
         <v>173</v>
       </c>
       <c r="C81" t="s">
-        <v>329</v>
-      </c>
-      <c r="D81" t="s">
-        <v>330</v>
+        <v>258</v>
+      </c>
+      <c r="D81" s="66" t="s">
+        <v>259</v>
       </c>
       <c r="E81" t="b">
         <v>0</v>
@@ -8187,8 +8191,8 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:F81">
-    <sortCondition ref="A1:A1048576"/>
-    <sortCondition ref="B1:B1048576"/>
+    <sortCondition ref="B11:B81"/>
+    <sortCondition ref="C11:C81"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>